<commit_message>
updated based on Ajit's feedback
</commit_message>
<xml_diff>
--- a/public/Systems.xlsx
+++ b/public/Systems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilesh.heda\code\Sagar\rule-editor\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DAF01E-C6E0-44B2-845C-766FA39E3B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8152E26C-8F83-447E-9120-D04B6E85DE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28B2B8D7-8A39-8645-A9B0-54D055B01E4B}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15708" windowHeight="12336" xr2:uid="{28B2B8D7-8A39-8645-A9B0-54D055B01E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
   <si>
     <t>Platform Service</t>
   </si>
@@ -137,27 +137,9 @@
     <t>ESB (Enterprise Service Bus)</t>
   </si>
   <si>
-    <t>RDIP</t>
-  </si>
-  <si>
-    <t>(SAP-RFC,IDOC/Kafka/ API)</t>
-  </si>
-  <si>
-    <t>Platform Gateway</t>
-  </si>
-  <si>
-    <t>(API/Kafka/SAP/GRPC/Temporal/TIBCO)</t>
-  </si>
-  <si>
-    <t>SCM Kafka</t>
-  </si>
-  <si>
     <t>API Gateway</t>
   </si>
   <si>
-    <t>Treafik / RDIP</t>
-  </si>
-  <si>
     <t>Login Service </t>
   </si>
   <si>
@@ -212,9 +194,6 @@
     <t xml:space="preserve">SAP WM, Shipsy WM, Addverb WM, Viculum WM, RWOS WM </t>
   </si>
   <si>
-    <t xml:space="preserve">WMS </t>
-  </si>
-  <si>
     <t xml:space="preserve">Darkstore management System </t>
   </si>
   <si>
@@ -260,98 +239,134 @@
     <t xml:space="preserve">Rover / Shipsy </t>
   </si>
   <si>
-    <t xml:space="preserve">Warehouse Automation
+    <t>EwayBill, manifestation, Trip data, Vahan Portal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rover / Shipsy / SAP Ztrip </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manpower planning, Trip Management, VAS Services </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grab </t>
+  </si>
+  <si>
+    <t>Transport Mgmt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trip Planning and Management, hub Management, Vehicle planning, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Costing, (Manpower/ Vehicle / Carrier), Payment and Reconcilaiton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qbill, SAP RP5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track and Trace </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS tracking, Shipment tracking, Trip Tracking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jio Humsafar, Shipsy, Rover, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Integration Adapter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMS / Hana / RUI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE / Sandstorm / JCP </t>
+  </si>
+  <si>
+    <t>Picking, Packing, QC, Returns, Receiving, Dispatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan vs Actual monitoring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emails </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP/ Herald / ROMS </t>
+  </si>
+  <si>
+    <t>RRA, Clickhouse, Databricks, Tableu</t>
+  </si>
+  <si>
+    <t>Common UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herald / ROMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herald / ROMS / SAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herald / Fynd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration with Various Storefront (JCP, Marketplace Adapters, Internal SF) and SCM, VMS, 3rd Party ERPs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wareshouse Management 
 </t>
   </si>
   <si>
-    <t xml:space="preserve">WCS / WES - PLC Sorter, PTL, Cubi-scan, DWS, RFID,  </t>
-  </si>
-  <si>
-    <t>EwayBill, manifestation, Trip data, Vahan Portal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rover / Shipsy / SAP Ztrip </t>
-  </si>
-  <si>
-    <t>Last Mile / hyperlocal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manpower planning, Trip Management, VAS Services </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grab </t>
-  </si>
-  <si>
-    <t>Transport Mgmt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trip Planning and Management, hub Management, Vehicle planning, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costing </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Costing, (Manpower/ Vehicle / Carrier), Payment and Reconcilaiton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qbill, SAP RP5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Track and Trace </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS tracking, Shipment tracking, Trip Tracking </t>
-  </si>
-  <si>
-    <t xml:space="preserve">jio Humsafar, Shipsy, Rover, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">External Integration Adapter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMS / Hana / RUI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE / Sandstorm / JCP </t>
-  </si>
-  <si>
-    <t>Picking, Packing, QC, Returns, Receiving, Dispatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan vs Actual monitoring </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emails </t>
-  </si>
-  <si>
-    <t>SAP Financial</t>
-  </si>
-  <si>
-    <t>POSDTA, SAP financial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP/ Herald / ROMS </t>
-  </si>
-  <si>
-    <t>RRA, Clickhouse, Databricks, Tableu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data marts, Reporting </t>
-  </si>
-  <si>
-    <t>Common UI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herald / ROMS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herald / ROMS / SAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herald / Fynd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integration with Various Storefront (JCP, Marketplace Adapters, Internal SF) and SCM, VMS, 3rd Party ERPs. </t>
+    <t xml:space="preserve">Picking, Packing, QC, Returns, Receiving, Dispatch, Bin Management </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treafik, RDIP </t>
+  </si>
+  <si>
+    <t>Herald CLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform Integration Layer </t>
+  </si>
+  <si>
+    <t>Herald Gateway, RDIP</t>
+  </si>
+  <si>
+    <t>Event processor, Rule Engine, Transfomation and routing (API/Kafka/SAP/GRPC/Temporal/TIBCO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http Api gateway, rate limiting, Traffic ingress </t>
+  </si>
+  <si>
+    <t>Data marts, Reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting platform </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse Automation &amp; Execution </t>
+  </si>
+  <si>
+    <t>WCS, WES, PLC Sorter, PTL, Cubi-scan, DWS, RFID,  Robotics</t>
+  </si>
+  <si>
+    <t>SAP FI/CO</t>
+  </si>
+  <si>
+    <t>POSDTA, SAP FI/CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution Apps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picking, Packing, QC, Returns, Receiving, PI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP, Herald, ROMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Mile / hyperlocal / Quick commerce </t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -411,9 +426,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06262CDC-C76D-764A-8F54-3F814DB2115F}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -781,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,66 +815,66 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -886,10 +898,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -900,18 +912,18 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -927,10 +939,10 @@
     </row>
     <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -968,43 +980,43 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1014,24 +1026,24 @@
     </row>
     <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1039,54 +1051,54 @@
         <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1094,35 +1106,48 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="5" t="s">
+    <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1132,18 +1157,18 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1153,10 +1178,13 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1164,47 +1192,40 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>34</v>
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>36</v>
+        <v>99</v>
+      </c>
+      <c r="C60" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>40</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B45:B46"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 2 based on Ajit's feedback
</commit_message>
<xml_diff>
--- a/public/Systems.xlsx
+++ b/public/Systems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilesh.heda\code\Sagar\rule-editor\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8152E26C-8F83-447E-9120-D04B6E85DE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B915A935-BECB-46BA-9D82-8AA6E578422A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15708" windowHeight="12336" xr2:uid="{28B2B8D7-8A39-8645-A9B0-54D055B01E4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Platform Service</t>
   </si>
@@ -96,18 +96,6 @@
   </si>
   <si>
     <t>Financial Services</t>
-  </si>
-  <si>
-    <t>Invoicing</t>
-  </si>
-  <si>
-    <t>( Invoicing / Sales Posting / Credit Note / Debit Note )</t>
-  </si>
-  <si>
-    <t>( Payment Ledger/ Refund Ledger)</t>
-  </si>
-  <si>
-    <t>Refund Services </t>
   </si>
   <si>
     <t>(Herald/Sterling/Fynd)</t>
@@ -367,6 +355,21 @@
   </si>
   <si>
     <t xml:space="preserve">Last Mile / hyperlocal / Quick commerce </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Management </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory Management and Ledger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP IM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoicing &amp; Refund Services </t>
+  </si>
+  <si>
+    <t>Invoicing / Sales Posting / Credit Note / Debit Note, Payment Ledger, Refund Ledger</t>
   </si>
 </sst>
 </file>
@@ -763,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06262CDC-C76D-764A-8F54-3F814DB2115F}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -793,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -815,66 +818,66 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -890,7 +893,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -898,10 +901,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -912,18 +915,18 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -939,10 +942,10 @@
     </row>
     <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -953,276 +956,276 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
         <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
         <v>62</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C59" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>